<commit_message>
JNG-2526: add checking of reviewRequired flag and correct test cases
</commit_message>
<xml_diff>
--- a/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
+++ b/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CasesOriginal" sheetId="1" state="visible" r:id="rId2"/>
@@ -1152,11 +1152,11 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D33" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -15149,13 +15149,13 @@
   </sheetPr>
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
@@ -15320,7 +15320,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>132</v>
@@ -15355,7 +15355,7 @@
         <v>17</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>19</v>
@@ -15390,7 +15390,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>19</v>
@@ -16976,7 +16976,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17099,7 +17099,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17207,11 +17207,11 @@
   </sheetPr>
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K54" activeCellId="0" sqref="K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="15.15"/>
@@ -30566,7 +30566,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="33" t="s">

</xml_diff>

<commit_message>
JNG-2526: fix review required of create field (review required only if field is mandatory)
</commit_message>
<xml_diff>
--- a/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
+++ b/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="176">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -1156,7 +1156,7 @@
       <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -15150,12 +15150,12 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
@@ -16191,7 +16191,9 @@
       <c r="F30" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="23"/>
+      <c r="G30" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="H30" s="23" t="s">
         <v>19</v>
       </c>
@@ -16976,7 +16978,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17099,7 +17101,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17207,11 +17209,11 @@
   </sheetPr>
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K54" activeCellId="0" sqref="K54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="15.15"/>
@@ -17469,9 +17471,7 @@
       <c r="J14" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="40" t="s">
-        <v>174</v>
-      </c>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
@@ -17742,9 +17742,7 @@
       <c r="J29" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="K29" s="40" t="s">
-        <v>174</v>
-      </c>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
@@ -17881,9 +17879,7 @@
       <c r="J36" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="K36" s="40" t="s">
-        <v>174</v>
-      </c>
+      <c r="K36" s="40"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="38" t="s">
@@ -30566,7 +30562,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="33" t="s">

</xml_diff>

<commit_message>
JNG-2526: make reviewRequired flag true for all CreateFieldOperations
</commit_message>
<xml_diff>
--- a/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
+++ b/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="175">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -1140,10 +1140,10 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="1" sqref="J1 D44"/>
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -15139,10 +15139,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G31" activeCellId="1" sqref="J1 G31"/>
+      <selection pane="bottomLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
@@ -16962,10 +16962,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="J1 A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17085,10 +17085,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="J1 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17196,11 +17196,11 @@
   </sheetPr>
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J36" activeCellId="0" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="15.15"/>
@@ -17443,7 +17443,9 @@
       <c r="I14" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J14" s="39"/>
+      <c r="J14" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="37" t="s">
@@ -17699,7 +17701,9 @@
       <c r="I29" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J29" s="39"/>
+      <c r="J29" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="37" t="s">
@@ -17829,7 +17833,9 @@
       <c r="I36" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J36" s="39"/>
+      <c r="J36" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="37" t="s">
@@ -29544,10 +29550,10 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="J1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
   </cols>

</xml_diff>

<commit_message>
JNG-2526: make reviewRequired flag true for all type changes, remove isString flag and fix previous wrong commit (newly created field must be reviewed if they are mandatory)
</commit_message>
<xml_diff>
--- a/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
+++ b/model-test/src/test/resources/RdbmsIncrementalTests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="175">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -1140,10 +1140,10 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
+      <selection pane="topLeft" activeCell="D44" activeCellId="1" sqref="33:33 D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -15137,12 +15137,12 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="C32" activeCellId="1" sqref="33:33 C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
@@ -16962,10 +16962,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="33:33 A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17085,10 +17085,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="33:33 A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -17196,11 +17196,11 @@
   </sheetPr>
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J36" activeCellId="0" sqref="J36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="33:33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="15.15"/>
@@ -17283,7 +17283,9 @@
       <c r="G4" s="38"/>
       <c r="H4" s="38"/>
       <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
+      <c r="J4" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="37" t="s">
@@ -17443,9 +17445,7 @@
       <c r="I14" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J14" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="J14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="37" t="s">
@@ -17479,7 +17479,9 @@
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
+      <c r="J16" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="37" t="s">
@@ -17701,9 +17703,7 @@
       <c r="I29" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J29" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="37" t="s">
@@ -17833,9 +17833,7 @@
       <c r="I36" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J36" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="37" t="s">
@@ -17995,9 +17993,7 @@
       <c r="I46" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J46" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="37" t="s">
@@ -29550,10 +29546,10 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="33:33 I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
   </cols>

</xml_diff>